<commit_message>
update intact policy search
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dev\Python-Automations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0405E9E-7D43-483D-9731-40B1B6CA66E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13020" yWindow="1530" windowWidth="18000" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13020" yWindow="1530" windowWidth="18000" windowHeight="12930"/>
   </bookViews>
   <sheets>
     <sheet name="File Completion Tool" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +35,6 @@
     <t>Event:</t>
   </si>
   <si>
-    <t>Auto Renewal Letter</t>
-  </si>
-  <si>
     <t>CSR Name for Auto Renewal Letter:</t>
   </si>
   <si>
@@ -76,12 +72,15 @@
   </si>
   <si>
     <t>Risk Address:</t>
+  </si>
+  <si>
+    <t>Sort Renewal List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,9 +260,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -274,6 +270,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -555,11 +554,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,10 +573,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="11"/>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,15 +586,15 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="13"/>
+      <c r="B3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12"/>
       <c r="D3" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -606,7 +605,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3"/>
     </row>
@@ -615,13 +614,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -634,66 +633,66 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -713,10 +712,10 @@
     <mergeCell ref="B22:C22"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{0C358B17-816B-4821-A717-B4455615BAFA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
       <formula1>"condo, home, rented_dwelling, rented_condo, tenant"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:C3" xr:uid="{DA8A6AF5-1B0C-4C9C-A743-0DFEC40235AC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:C3">
       <formula1>"Auto Renewal Letter, Manual Renewal Letter, Sort Renewal List"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>